<commit_message>
Update AEO2023 IRA 5cenario outputs by OnL 07-25-23.xlsx
</commit_message>
<xml_diff>
--- a/data-raw/model-runs/AEO2023 IRA 5cenario outputs by OnL 07-25-23.xlsx
+++ b/data-raw/model-runs/AEO2023 IRA 5cenario outputs by OnL 07-25-23.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sweisberg\Documents\LEEP\data-raw\model-runs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{091DA2DA-8669-4D6B-8142-2AD95B0E1F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E31A9C7-98CE-406D-9EFB-0187B9CBB071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-6120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD14A334-AA51-4896-9CCE-196B3E25482D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AD14A334-AA51-4896-9CCE-196B3E25482D}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$AJ$557</definedName>
     <definedName name="FTAB_ID">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2751" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2761" uniqueCount="318">
   <si>
     <t>Model</t>
   </si>
@@ -990,6 +991,9 @@
   <si>
     <t>Capacity Retirements|Electricity|Wind</t>
   </si>
+  <si>
+    <t>Emissions|CO2</t>
+  </si>
 </sst>
 </file>
 
@@ -1063,7 +1067,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1092,6 +1096,8 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1408,13 +1414,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5167365A-4B3B-4D19-AB36-3F431585B511}">
-  <dimension ref="A1:AJ557"/>
+  <dimension ref="A1:AJ559"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A536" workbookViewId="0">
+      <selection activeCell="B560" sqref="B560"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="64.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
@@ -61652,6 +61662,288 @@
       </c>
       <c r="AJ557" s="5">
         <v>0</v>
+      </c>
+    </row>
+    <row r="558" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A558" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B558" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C558" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="D558" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="E558" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F558" s="17">
+        <f>F31+F53</f>
+        <v>0</v>
+      </c>
+      <c r="G558" s="17">
+        <f t="shared" ref="G558:AJ558" si="2">G31+G53</f>
+        <v>0</v>
+      </c>
+      <c r="H558" s="17">
+        <f t="shared" si="2"/>
+        <v>4865.1807749999998</v>
+      </c>
+      <c r="I558" s="17">
+        <f t="shared" si="2"/>
+        <v>4762.5441680000004</v>
+      </c>
+      <c r="J558" s="17">
+        <f t="shared" si="2"/>
+        <v>4695.3848509999998</v>
+      </c>
+      <c r="K558" s="17">
+        <f t="shared" si="2"/>
+        <v>4611.5313919999999</v>
+      </c>
+      <c r="L558" s="17">
+        <f t="shared" si="2"/>
+        <v>4569.3506170000001</v>
+      </c>
+      <c r="M558" s="17">
+        <f t="shared" si="2"/>
+        <v>4530.8830539999999</v>
+      </c>
+      <c r="N558" s="17">
+        <f t="shared" si="2"/>
+        <v>4505.2794139999996</v>
+      </c>
+      <c r="O558" s="17">
+        <f t="shared" si="2"/>
+        <v>4479.9688310000001</v>
+      </c>
+      <c r="P558" s="17">
+        <f t="shared" si="2"/>
+        <v>4436.1795170000005</v>
+      </c>
+      <c r="Q558" s="17">
+        <f t="shared" si="2"/>
+        <v>4386.0622209999992</v>
+      </c>
+      <c r="R558" s="17">
+        <f t="shared" si="2"/>
+        <v>4352.9353419999998</v>
+      </c>
+      <c r="S558" s="17">
+        <f t="shared" si="2"/>
+        <v>4341.0706</v>
+      </c>
+      <c r="T558" s="17">
+        <f t="shared" si="2"/>
+        <v>4332.8995649999997</v>
+      </c>
+      <c r="U558" s="17">
+        <f t="shared" si="2"/>
+        <v>4318.5328509999999</v>
+      </c>
+      <c r="V558" s="17">
+        <f t="shared" si="2"/>
+        <v>4300.0624640000005</v>
+      </c>
+      <c r="W558" s="17">
+        <f t="shared" si="2"/>
+        <v>4297.814402</v>
+      </c>
+      <c r="X558" s="17">
+        <f t="shared" si="2"/>
+        <v>4276.3921410000003</v>
+      </c>
+      <c r="Y558" s="17">
+        <f t="shared" si="2"/>
+        <v>4262.5982199999999</v>
+      </c>
+      <c r="Z558" s="17">
+        <f t="shared" si="2"/>
+        <v>4245.8689859999995</v>
+      </c>
+      <c r="AA558" s="17">
+        <f t="shared" si="2"/>
+        <v>4254.5650370000003</v>
+      </c>
+      <c r="AB558" s="17">
+        <f t="shared" si="2"/>
+        <v>4266.7690039999998</v>
+      </c>
+      <c r="AC558" s="17">
+        <f t="shared" si="2"/>
+        <v>4275.0003530000004</v>
+      </c>
+      <c r="AD558" s="17">
+        <f t="shared" si="2"/>
+        <v>4277.1535829999993</v>
+      </c>
+      <c r="AE558" s="17">
+        <f t="shared" si="2"/>
+        <v>4278.596571</v>
+      </c>
+      <c r="AF558" s="17">
+        <f t="shared" si="2"/>
+        <v>4285.6663010000002</v>
+      </c>
+      <c r="AG558" s="17">
+        <f t="shared" si="2"/>
+        <v>4288.5327239999997</v>
+      </c>
+      <c r="AH558" s="17">
+        <f t="shared" si="2"/>
+        <v>4289.5859139999993</v>
+      </c>
+      <c r="AI558" s="17">
+        <f t="shared" si="2"/>
+        <v>4304.7878430000001</v>
+      </c>
+      <c r="AJ558" s="17">
+        <f t="shared" si="2"/>
+        <v>4320.6721279999992</v>
+      </c>
+    </row>
+    <row r="559" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A559" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B559" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C559" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="D559" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="E559" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F559" s="17">
+        <f>F308+F331</f>
+        <v>4587.5389580000001</v>
+      </c>
+      <c r="G559" s="17">
+        <f t="shared" ref="G559:AJ559" si="3">G308+G331</f>
+        <v>4883.3729430000003</v>
+      </c>
+      <c r="H559" s="17">
+        <f t="shared" si="3"/>
+        <v>4864.6837880000003</v>
+      </c>
+      <c r="I559" s="17">
+        <f t="shared" si="3"/>
+        <v>4726.2107909999995</v>
+      </c>
+      <c r="J559" s="17">
+        <f t="shared" si="3"/>
+        <v>4674.8438399999995</v>
+      </c>
+      <c r="K559" s="17">
+        <f t="shared" si="3"/>
+        <v>4564.102887</v>
+      </c>
+      <c r="L559" s="17">
+        <f t="shared" si="3"/>
+        <v>4432.4653550000003</v>
+      </c>
+      <c r="M559" s="17">
+        <f t="shared" si="3"/>
+        <v>4290.4765420000003</v>
+      </c>
+      <c r="N559" s="17">
+        <f t="shared" si="3"/>
+        <v>4181.9763750000002</v>
+      </c>
+      <c r="O559" s="17">
+        <f t="shared" si="3"/>
+        <v>4084.3307569999997</v>
+      </c>
+      <c r="P559" s="17">
+        <f t="shared" si="3"/>
+        <v>4007.4891739999998</v>
+      </c>
+      <c r="Q559" s="17">
+        <f t="shared" si="3"/>
+        <v>3972.2999279999999</v>
+      </c>
+      <c r="R559" s="17">
+        <f t="shared" si="3"/>
+        <v>3958.6173670000003</v>
+      </c>
+      <c r="S559" s="17">
+        <f t="shared" si="3"/>
+        <v>3944.8042089999999</v>
+      </c>
+      <c r="T559" s="17">
+        <f t="shared" si="3"/>
+        <v>3921.258781</v>
+      </c>
+      <c r="U559" s="17">
+        <f t="shared" si="3"/>
+        <v>3904.6754209999999</v>
+      </c>
+      <c r="V559" s="17">
+        <f t="shared" si="3"/>
+        <v>3892.6559729999999</v>
+      </c>
+      <c r="W559" s="17">
+        <f t="shared" si="3"/>
+        <v>3889.5545729999999</v>
+      </c>
+      <c r="X559" s="17">
+        <f t="shared" si="3"/>
+        <v>3878.2416079999998</v>
+      </c>
+      <c r="Y559" s="17">
+        <f t="shared" si="3"/>
+        <v>3877.781234</v>
+      </c>
+      <c r="Z559" s="17">
+        <f t="shared" si="3"/>
+        <v>3878.180421</v>
+      </c>
+      <c r="AA559" s="17">
+        <f t="shared" si="3"/>
+        <v>3887.0041840000004</v>
+      </c>
+      <c r="AB559" s="17">
+        <f t="shared" si="3"/>
+        <v>3897.270411</v>
+      </c>
+      <c r="AC559" s="17">
+        <f t="shared" si="3"/>
+        <v>3901.5770969999999</v>
+      </c>
+      <c r="AD559" s="17">
+        <f t="shared" si="3"/>
+        <v>3909.2728999999999</v>
+      </c>
+      <c r="AE559" s="17">
+        <f t="shared" si="3"/>
+        <v>3913.6458480000001</v>
+      </c>
+      <c r="AF559" s="17">
+        <f t="shared" si="3"/>
+        <v>3909.3941530000002</v>
+      </c>
+      <c r="AG559" s="17">
+        <f t="shared" si="3"/>
+        <v>3920.3457490000001</v>
+      </c>
+      <c r="AH559" s="17">
+        <f t="shared" si="3"/>
+        <v>3925.1035549999997</v>
+      </c>
+      <c r="AI559" s="17">
+        <f t="shared" si="3"/>
+        <v>3929.8643379999999</v>
+      </c>
+      <c r="AJ559" s="17">
+        <f t="shared" si="3"/>
+        <v>3942.922047</v>
       </c>
     </row>
   </sheetData>
@@ -61903,15 +62195,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f856ad2f-e557-432f-a854-14e859f15249" xsi:nil="true"/>
@@ -61920,6 +62203,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -61942,14 +62234,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3684B28-2848-4B39-8D9D-44169DB678D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DD9A1D7-15DD-4119-892B-3556E77B3410}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="f856ad2f-e557-432f-a854-14e859f15249"/>
@@ -61964,4 +62248,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3684B28-2848-4B39-8D9D-44169DB678D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>